<commit_message>
sawg-distal-colon: fix missing local conventions
</commit_message>
<xml_diff>
--- a/sawg-distal-colon/source/sawg-distal-colon.xlsx
+++ b/sawg-distal-colon/source/sawg-distal-colon.xlsx
@@ -11,6 +11,7 @@
     <sheet state="visible" name="nodes" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="groups" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="publications" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="localConventions" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="942">
   <si>
     <t>id</t>
   </si>
@@ -2813,13 +2814,85 @@
   </si>
   <si>
     <t>https://pubmed.ncbi.nlm.nih.gov/4044909/</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>namespace</t>
+  </si>
+  <si>
+    <t>UBERON</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UBERON_</t>
+  </si>
+  <si>
+    <t>CHEBI</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_</t>
+  </si>
+  <si>
+    <t>FMA</t>
+  </si>
+  <si>
+    <t>http://purl.org/sig/ont/fma/fma</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GO_</t>
+  </si>
+  <si>
+    <t>ILX</t>
+  </si>
+  <si>
+    <t>http://uri.interlex.org/base/ilx_</t>
+  </si>
+  <si>
+    <t>NLX</t>
+  </si>
+  <si>
+    <t>http://uri.neuinfo.org/nif/nifstd/nlx_</t>
+  </si>
+  <si>
+    <t>SAO</t>
+  </si>
+  <si>
+    <t>http://uri.neuinfo.org/nif/nifstd/sao</t>
+  </si>
+  <si>
+    <t>PMID</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/pubmed/</t>
+  </si>
+  <si>
+    <t>EMAPA</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EMAPA_</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CL_</t>
+  </si>
+  <si>
+    <t>NCBITaxon</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCBITaxon_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+  <fonts count="21">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2898,6 +2971,21 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2925,7 +3013,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border/>
     <border>
       <left style="thin">
@@ -2938,11 +3026,25 @@
         <color rgb="FF000000"/>
       </top>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="89">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3195,6 +3297,21 @@
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3232,6 +3349,10 @@
 </file>
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -11166,4 +11287,416 @@
   </hyperlinks>
   <drawing r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="84" t="s">
+        <v>918</v>
+      </c>
+      <c r="B1" s="84" t="s">
+        <v>919</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="19" t="s">
+        <v>920</v>
+      </c>
+      <c r="B2" s="85" t="s">
+        <v>921</v>
+      </c>
+      <c r="C2" s="86"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="19" t="s">
+        <v>922</v>
+      </c>
+      <c r="B3" s="87" t="s">
+        <v>923</v>
+      </c>
+      <c r="C3" s="86"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="19" t="s">
+        <v>924</v>
+      </c>
+      <c r="B4" s="87" t="s">
+        <v>925</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="19" t="s">
+        <v>926</v>
+      </c>
+      <c r="B5" s="87" t="s">
+        <v>927</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="19" t="s">
+        <v>928</v>
+      </c>
+      <c r="B6" s="87" t="s">
+        <v>929</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="19" t="s">
+        <v>930</v>
+      </c>
+      <c r="B7" s="87" t="s">
+        <v>931</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="19" t="s">
+        <v>932</v>
+      </c>
+      <c r="B8" s="87" t="s">
+        <v>933</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="19" t="s">
+        <v>934</v>
+      </c>
+      <c r="B9" s="87" t="s">
+        <v>935</v>
+      </c>
+      <c r="C9" s="86"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="19" t="s">
+        <v>936</v>
+      </c>
+      <c r="B10" s="87" t="s">
+        <v>937</v>
+      </c>
+      <c r="C10" s="86"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="19" t="s">
+        <v>938</v>
+      </c>
+      <c r="B11" s="87" t="s">
+        <v>939</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="15" t="s">
+        <v>940</v>
+      </c>
+      <c r="B12" s="88" t="s">
+        <v>941</v>
+      </c>
+      <c r="C12" s="86"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="B4"/>
+    <hyperlink r:id="rId4" ref="B5"/>
+    <hyperlink r:id="rId5" ref="B6"/>
+    <hyperlink r:id="rId6" ref="B7"/>
+    <hyperlink r:id="rId7" ref="B8"/>
+    <hyperlink r:id="rId8" ref="B9"/>
+    <hyperlink r:id="rId9" ref="B10"/>
+    <hyperlink r:id="rId10" ref="B11"/>
+    <hyperlink r:id="rId11" ref="B12"/>
+  </hyperlinks>
+  <drawing r:id="rId12"/>
+</worksheet>
 </file>
</xml_diff>